<commit_message>
Se añaden capturas para readme, se amplica el readme. Se añade funcionalidad para dejar marca de leído sin responder, se añade funcionalidad de responder automáticamente basado en respuesta dejadas en un excel.
</commit_message>
<xml_diff>
--- a/Archivos/Comentarios.xlsx
+++ b/Archivos/Comentarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_EADF97BC9FACEB5C6EA9F2648D13A887F5320AF2" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2B2BC15-F65B-4076-A2FA-838598939154}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_286BF6A074AD6B509EB8F15341F0A641F532AA94" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE241DA1-3016-4D2E-AA08-81EBA4E5B3DE}"/>
   <x:bookViews>
     <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="313">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="315">
   <x:si>
     <x:t>Nombre</x:t>
   </x:si>
@@ -39,40 +39,22 @@
     <x:t>Seguimiento</x:t>
   </x:si>
   <x:si>
-    <x:t>MoniCmpos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Excelente video!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>platzi.com/comentario/1031193/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>test</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jonathan Cardona Calderon</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Con el tarareo me lanzaron agua por que pensaron que andaba delirando pero quede limpio que era lo importante jejeje </x:t>
-  </x:si>
-  <x:si>
-    <x:t>platzi.com/comentario/1356925/</x:t>
+    <x:t>UltimaRespuesta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Midelar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Es hora de limpiar el teclado con alcohol…</x:t>
+  </x:si>
+  <x:si>
+    <x:t>platzi.com/comentario/1356143/</x:t>
   </x:si>
   <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>MIGUEL ANGEL DELGADO ARPITA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Es hora de limpiar el teclado con alcohol…</x:t>
-  </x:si>
-  <x:si>
-    <x:t>platzi.com/comentario/1356143/</x:t>
+    <x:t>Esto es una prueba de un Robot, disculpa las molestías.</x:t>
   </x:si>
   <x:si>
     <x:t>Jose Antonio Rojas Ollarves</x:t>
@@ -591,6 +573,33 @@
     <x:t>13</x:t>
   </x:si>
   <x:si>
+    <x:t>Necesito uno de esos!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MoniCmpos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Excelente video!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>platzi.com/comentario/1031193/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jonathan Cardona Calderon</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Con el tarareo me lanzaron agua por que pensaron que andaba delirando pero quede limpio que era lo importante jejeje </x:t>
+  </x:si>
+  <x:si>
+    <x:t>platzi.com/comentario/1356925/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>prueba</x:t>
+  </x:si>
+  <x:si>
     <x:t>Nicolas Palavecino</x:t>
   </x:si>
   <x:si>
@@ -598,9 +607,6 @@
   </x:si>
   <x:si>
     <x:t>platzi.com/comentario/1279822/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2</x:t>
   </x:si>
   <x:si>
     <x:t>Jorge Francisco Onasis Ramos Nava</x:t>
@@ -1025,7 +1031,8 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1335,865 +1342,855 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E60"/>
+  <x:dimension ref="A1:F59"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="B17" sqref="B17 B17:B17"/>
+      <x:selection activeCell="F3" sqref="F3 F3:F3"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="10.561875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="21.961719" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="35.285156" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="17.855469" style="1" customWidth="1"/>
-    <x:col min="3" max="3" width="30.285156" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="5" max="5" width="12.285156" style="1" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="35.285156" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="65.140625" style="2" customWidth="1"/>
+    <x:col min="3" max="3" width="30.285156" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="5" max="5" width="12.285156" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="6" max="6" width="16.140625" style="2" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="1" t="s">
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="2" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="1" t="s">
+      <x:c r="B1" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="1" t="s">
+      <x:c r="C1" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="1" t="s">
+      <x:c r="D1" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="1" t="s">
+      <x:c r="E1" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="1" t="s">
+      <x:c r="F1" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B2" s="1" t="s">
+    </x:row>
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="2" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C2" s="1" t="s">
+      <x:c r="B2" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D2" s="1" t="s">
+      <x:c r="C2" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="E2" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="1" t="s">
+      <x:c r="D2" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="B3" s="1" t="s">
+    </x:row>
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="2" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C3" s="1" t="s">
+      <x:c r="B3" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D3" s="1" t="s">
+      <x:c r="C3" s="2" t="s">
         <x:v>13</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="1" t="s">
+      <x:c r="D3" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="2" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="B4" s="1" t="s">
+      <x:c r="B4" s="2" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="C4" s="1" t="s">
+      <x:c r="C4" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="D4" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="1" t="s">
+      <x:c r="D4" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="B5" s="1" t="s">
+      <x:c r="B5" s="2" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="C5" s="1" t="s">
+      <x:c r="C5" s="2" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="D5" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="1" t="s">
+      <x:c r="D5" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="2" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="B6" s="1" t="s">
+      <x:c r="B6" s="2" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C6" s="1" t="s">
+      <x:c r="C6" s="2" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="D6" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="1" t="s">
+      <x:c r="D6" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="2" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B7" s="1" t="s">
+      <x:c r="B7" s="2" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="C7" s="1" t="s">
+      <x:c r="C7" s="2" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="D7" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="1" t="s">
+      <x:c r="D7" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B8" s="1" t="s">
+      <x:c r="C8" s="2" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="C8" s="1" t="s">
+      <x:c r="D8" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="2" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="D8" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="1" t="s">
+      <x:c r="B9" s="2" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="B9" s="1" t="s">
+      <x:c r="C9" s="2" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="C9" s="1" t="s">
+      <x:c r="D9" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="2" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="D9" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="1" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="B10" s="1" t="s">
+      <x:c r="B10" s="2" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="C10" s="1" t="s">
+      <x:c r="C10" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="D10" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="1" t="s">
+      <x:c r="D10" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="2" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="B11" s="1" t="s">
+      <x:c r="B11" s="2" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="C11" s="1" t="s">
+      <x:c r="C11" s="2" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="D11" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="1" t="s">
+      <x:c r="D11" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="2" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="B12" s="1" t="s">
+      <x:c r="B12" s="2" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="C12" s="1" t="s">
+      <x:c r="C12" s="2" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="D12" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A13" s="1" t="s">
+      <x:c r="D12" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="2" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="B13" s="1" t="s">
+      <x:c r="B13" s="2" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="C13" s="1" t="s">
+      <x:c r="C13" s="2" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="D13" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A14" s="1" t="s">
+      <x:c r="D13" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="2" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="B14" s="1" t="s">
+      <x:c r="B14" s="2" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="C14" s="1" t="s">
+      <x:c r="C14" s="2" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="D14" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A15" s="1" t="s">
+      <x:c r="D14" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="2" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="B15" s="1" t="s">
+      <x:c r="B15" s="2" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="C15" s="1" t="s">
+      <x:c r="C15" s="2" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="D15" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A16" s="1" t="s">
+      <x:c r="D15" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A16" s="2" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="B16" s="1" t="s">
+      <x:c r="B16" s="2" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="C16" s="1" t="s">
+      <x:c r="C16" s="2" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="D16" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A17" s="1" t="s">
+      <x:c r="D16" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A17" s="2" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="B17" s="1" t="s">
+      <x:c r="B17" s="2" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="C17" s="1" t="s">
+      <x:c r="C17" s="2" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="D17" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A18" s="1" t="s">
+      <x:c r="D17" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A18" s="2" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="B18" s="1" t="s">
+      <x:c r="B18" s="2" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="C18" s="1" t="s">
+      <x:c r="C18" s="2" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="D18" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A19" s="1" t="s">
+      <x:c r="D18" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A19" s="2" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="B19" s="1" t="s">
+      <x:c r="B19" s="2" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="C19" s="1" t="s">
+      <x:c r="C19" s="2" t="s">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="D19" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A20" s="1" t="s">
+      <x:c r="D19" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A20" s="2" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="B20" s="1" t="s">
+      <x:c r="B20" s="2" t="s">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="C20" s="1" t="s">
+      <x:c r="C20" s="2" t="s">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="D20" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A21" s="1" t="s">
+      <x:c r="D20" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A21" s="2" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="B21" s="1" t="s">
+      <x:c r="B21" s="2" t="s">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="C21" s="1" t="s">
+      <x:c r="C21" s="2" t="s">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="D21" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A22" s="1" t="s">
+      <x:c r="D21" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A22" s="2" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="B22" s="1" t="s">
+      <x:c r="B22" s="2" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="C22" s="1" t="s">
+      <x:c r="C22" s="2" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="D22" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A23" s="1" t="s">
+      <x:c r="D22" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A23" s="2" t="s">
         <x:v>70</x:v>
       </x:c>
-      <x:c r="B23" s="1" t="s">
+      <x:c r="B23" s="2" t="s">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="C23" s="1" t="s">
+      <x:c r="C23" s="2" t="s">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="D23" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A24" s="1" t="s">
+      <x:c r="D23" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A24" s="2" t="s">
         <x:v>73</x:v>
       </x:c>
-      <x:c r="B24" s="1" t="s">
+      <x:c r="B24" s="2" t="s">
         <x:v>74</x:v>
       </x:c>
-      <x:c r="C24" s="1" t="s">
+      <x:c r="C24" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D24" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A25" s="1" t="s">
+      <x:c r="D24" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A25" s="2" t="s">
         <x:v>76</x:v>
       </x:c>
-      <x:c r="B25" s="1" t="s">
+      <x:c r="B25" s="2" t="s">
         <x:v>77</x:v>
       </x:c>
-      <x:c r="C25" s="1" t="s">
+      <x:c r="C25" s="2" t="s">
         <x:v>78</x:v>
       </x:c>
-      <x:c r="D25" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A26" s="1" t="s">
+      <x:c r="D25" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A26" s="2" t="s">
         <x:v>79</x:v>
       </x:c>
-      <x:c r="B26" s="1" t="s">
+      <x:c r="B26" s="2" t="s">
         <x:v>80</x:v>
       </x:c>
-      <x:c r="C26" s="1" t="s">
+      <x:c r="C26" s="2" t="s">
         <x:v>81</x:v>
       </x:c>
-      <x:c r="D26" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A27" s="1" t="s">
+      <x:c r="D26" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A27" s="2" t="s">
         <x:v>82</x:v>
       </x:c>
-      <x:c r="B27" s="1" t="s">
+      <x:c r="B27" s="2" t="s">
         <x:v>83</x:v>
       </x:c>
-      <x:c r="C27" s="1" t="s">
+      <x:c r="C27" s="2" t="s">
         <x:v>84</x:v>
       </x:c>
-      <x:c r="D27" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A28" s="1" t="s">
+      <x:c r="D27" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A28" s="2" t="s">
         <x:v>85</x:v>
       </x:c>
-      <x:c r="B28" s="1" t="s">
+      <x:c r="B28" s="2" t="s">
         <x:v>86</x:v>
       </x:c>
-      <x:c r="C28" s="1" t="s">
+      <x:c r="C28" s="2" t="s">
         <x:v>87</x:v>
       </x:c>
-      <x:c r="D28" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A29" s="1" t="s">
+      <x:c r="D28" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A29" s="2" t="s">
         <x:v>88</x:v>
       </x:c>
-      <x:c r="B29" s="1" t="s">
+      <x:c r="B29" s="2" t="s">
         <x:v>89</x:v>
       </x:c>
-      <x:c r="C29" s="1" t="s">
+      <x:c r="C29" s="2" t="s">
         <x:v>90</x:v>
       </x:c>
-      <x:c r="D29" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A30" s="1" t="s">
+      <x:c r="D29" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A30" s="2" t="s">
         <x:v>91</x:v>
       </x:c>
-      <x:c r="B30" s="1" t="s">
+      <x:c r="B30" s="2" t="s">
         <x:v>92</x:v>
       </x:c>
-      <x:c r="C30" s="1" t="s">
+      <x:c r="C30" s="2" t="s">
         <x:v>93</x:v>
       </x:c>
-      <x:c r="D30" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A31" s="1" t="s">
+      <x:c r="D30" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A31" s="2" t="s">
         <x:v>94</x:v>
       </x:c>
-      <x:c r="B31" s="1" t="s">
+      <x:c r="B31" s="2" t="s">
         <x:v>95</x:v>
       </x:c>
-      <x:c r="C31" s="1" t="s">
+      <x:c r="C31" s="2" t="s">
         <x:v>96</x:v>
       </x:c>
-      <x:c r="D31" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A32" s="1" t="s">
+      <x:c r="D31" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A32" s="2" t="s">
         <x:v>97</x:v>
       </x:c>
-      <x:c r="B32" s="1" t="s">
+      <x:c r="B32" s="2" t="s">
         <x:v>98</x:v>
       </x:c>
-      <x:c r="C32" s="1" t="s">
+      <x:c r="C32" s="2" t="s">
         <x:v>99</x:v>
       </x:c>
-      <x:c r="D32" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A33" s="1" t="s">
+      <x:c r="D32" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A33" s="2" t="s">
         <x:v>100</x:v>
       </x:c>
-      <x:c r="B33" s="1" t="s">
+      <x:c r="B33" s="2" t="s">
         <x:v>101</x:v>
       </x:c>
-      <x:c r="C33" s="1" t="s">
+      <x:c r="C33" s="2" t="s">
         <x:v>102</x:v>
       </x:c>
-      <x:c r="D33" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A34" s="1" t="s">
+      <x:c r="D33" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A34" s="2" t="s">
         <x:v>103</x:v>
       </x:c>
-      <x:c r="B34" s="1" t="s">
+      <x:c r="B34" s="2" t="s">
         <x:v>104</x:v>
       </x:c>
-      <x:c r="C34" s="1" t="s">
+      <x:c r="C34" s="2" t="s">
         <x:v>105</x:v>
       </x:c>
-      <x:c r="D34" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A35" s="1" t="s">
+      <x:c r="D34" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A35" s="2" t="s">
         <x:v>106</x:v>
       </x:c>
-      <x:c r="B35" s="1" t="s">
+      <x:c r="B35" s="2" t="s">
         <x:v>107</x:v>
       </x:c>
-      <x:c r="C35" s="1" t="s">
+      <x:c r="C35" s="2" t="s">
         <x:v>108</x:v>
       </x:c>
-      <x:c r="D35" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A36" s="1" t="s">
+      <x:c r="D35" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A36" s="2" t="s">
         <x:v>109</x:v>
       </x:c>
-      <x:c r="B36" s="1" t="s">
+      <x:c r="B36" s="2" t="s">
         <x:v>110</x:v>
       </x:c>
-      <x:c r="C36" s="1" t="s">
+      <x:c r="C36" s="2" t="s">
         <x:v>111</x:v>
       </x:c>
-      <x:c r="D36" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A37" s="1" t="s">
+      <x:c r="D36" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A37" s="2" t="s">
         <x:v>112</x:v>
       </x:c>
-      <x:c r="B37" s="1" t="s">
+      <x:c r="B37" s="2" t="s">
         <x:v>113</x:v>
       </x:c>
-      <x:c r="C37" s="1" t="s">
+      <x:c r="C37" s="2" t="s">
         <x:v>114</x:v>
       </x:c>
-      <x:c r="D37" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A38" s="1" t="s">
+      <x:c r="D37" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A38" s="2" t="s">
         <x:v>115</x:v>
       </x:c>
-      <x:c r="B38" s="1" t="s">
+      <x:c r="B38" s="2" t="s">
         <x:v>116</x:v>
       </x:c>
-      <x:c r="C38" s="1" t="s">
+      <x:c r="C38" s="2" t="s">
         <x:v>117</x:v>
       </x:c>
-      <x:c r="D38" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A39" s="1" t="s">
+      <x:c r="D38" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A39" s="2" t="s">
         <x:v>118</x:v>
       </x:c>
-      <x:c r="B39" s="1" t="s">
+      <x:c r="B39" s="2" t="s">
         <x:v>119</x:v>
       </x:c>
-      <x:c r="C39" s="1" t="s">
+      <x:c r="C39" s="2" t="s">
         <x:v>120</x:v>
       </x:c>
-      <x:c r="D39" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A40" s="1" t="s">
+      <x:c r="D39" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A40" s="2" t="s">
         <x:v>121</x:v>
       </x:c>
-      <x:c r="B40" s="1" t="s">
+      <x:c r="B40" s="2" t="s">
         <x:v>122</x:v>
       </x:c>
-      <x:c r="C40" s="1" t="s">
+      <x:c r="C40" s="2" t="s">
         <x:v>123</x:v>
       </x:c>
-      <x:c r="D40" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A41" s="1" t="s">
+      <x:c r="D40" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A41" s="2" t="s">
         <x:v>124</x:v>
       </x:c>
-      <x:c r="B41" s="1" t="s">
+      <x:c r="B41" s="2" t="s">
         <x:v>125</x:v>
       </x:c>
-      <x:c r="C41" s="1" t="s">
+      <x:c r="C41" s="2" t="s">
         <x:v>126</x:v>
       </x:c>
-      <x:c r="D41" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A42" s="1" t="s">
+      <x:c r="D41" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A42" s="2" t="s">
         <x:v>127</x:v>
       </x:c>
-      <x:c r="B42" s="1" t="s">
+      <x:c r="B42" s="2" t="s">
         <x:v>128</x:v>
       </x:c>
-      <x:c r="C42" s="1" t="s">
+      <x:c r="C42" s="2" t="s">
         <x:v>129</x:v>
       </x:c>
-      <x:c r="D42" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A43" s="1" t="s">
+      <x:c r="D42" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A43" s="2" t="s">
         <x:v>130</x:v>
       </x:c>
-      <x:c r="B43" s="1" t="s">
+      <x:c r="B43" s="2" t="s">
         <x:v>131</x:v>
       </x:c>
-      <x:c r="C43" s="1" t="s">
+      <x:c r="C43" s="2" t="s">
         <x:v>132</x:v>
       </x:c>
-      <x:c r="D43" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A44" s="1" t="s">
+      <x:c r="D43" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A44" s="2" t="s">
         <x:v>133</x:v>
       </x:c>
-      <x:c r="B44" s="1" t="s">
+      <x:c r="B44" s="2" t="s">
         <x:v>134</x:v>
       </x:c>
-      <x:c r="C44" s="1" t="s">
+      <x:c r="C44" s="2" t="s">
         <x:v>135</x:v>
       </x:c>
-      <x:c r="D44" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A45" s="1" t="s">
+      <x:c r="D44" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A45" s="2" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="B45" s="2" t="s">
         <x:v>136</x:v>
       </x:c>
-      <x:c r="B45" s="1" t="s">
+      <x:c r="C45" s="2" t="s">
         <x:v>137</x:v>
       </x:c>
-      <x:c r="C45" s="1" t="s">
+      <x:c r="D45" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A46" s="2" t="s">
         <x:v>138</x:v>
       </x:c>
-      <x:c r="D45" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A46" s="1" t="s">
+      <x:c r="B46" s="2" t="s">
         <x:v>139</x:v>
       </x:c>
-      <x:c r="B46" s="1" t="s">
+      <x:c r="C46" s="2" t="s">
         <x:v>140</x:v>
       </x:c>
-      <x:c r="C46" s="1" t="s">
+      <x:c r="D46" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A47" s="2" t="s">
         <x:v>141</x:v>
       </x:c>
-      <x:c r="D46" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A47" s="1" t="s">
-        <x:v>139</x:v>
-      </x:c>
-      <x:c r="B47" s="1" t="s">
+      <x:c r="B47" s="2" t="s">
         <x:v>142</x:v>
       </x:c>
-      <x:c r="C47" s="1" t="s">
+      <x:c r="C47" s="2" t="s">
         <x:v>143</x:v>
       </x:c>
-      <x:c r="D47" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A48" s="1" t="s">
+      <x:c r="D47" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A48" s="2" t="s">
         <x:v>144</x:v>
       </x:c>
-      <x:c r="B48" s="1" t="s">
+      <x:c r="B48" s="2" t="s">
         <x:v>145</x:v>
       </x:c>
-      <x:c r="C48" s="1" t="s">
+      <x:c r="C48" s="2" t="s">
         <x:v>146</x:v>
       </x:c>
-      <x:c r="D48" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A49" s="1" t="s">
+      <x:c r="D48" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A49" s="2" t="s">
         <x:v>147</x:v>
       </x:c>
-      <x:c r="B49" s="1" t="s">
+      <x:c r="B49" s="2" t="s">
         <x:v>148</x:v>
       </x:c>
-      <x:c r="C49" s="1" t="s">
+      <x:c r="C49" s="2" t="s">
         <x:v>149</x:v>
       </x:c>
-      <x:c r="D49" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A50" s="1" t="s">
+      <x:c r="D49" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A50" s="2" t="s">
         <x:v>150</x:v>
       </x:c>
-      <x:c r="B50" s="1" t="s">
+      <x:c r="B50" s="2" t="s">
         <x:v>151</x:v>
       </x:c>
-      <x:c r="C50" s="1" t="s">
+      <x:c r="C50" s="2" t="s">
         <x:v>152</x:v>
       </x:c>
-      <x:c r="D50" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A51" s="1" t="s">
+      <x:c r="D50" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A51" s="2" t="s">
         <x:v>153</x:v>
       </x:c>
-      <x:c r="B51" s="1" t="s">
+      <x:c r="B51" s="2" t="s">
         <x:v>154</x:v>
       </x:c>
-      <x:c r="C51" s="1" t="s">
+      <x:c r="C51" s="2" t="s">
         <x:v>155</x:v>
       </x:c>
-      <x:c r="D51" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A52" s="1" t="s">
+      <x:c r="D51" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A52" s="2" t="s">
         <x:v>156</x:v>
       </x:c>
-      <x:c r="B52" s="1" t="s">
+      <x:c r="B52" s="2" t="s">
         <x:v>157</x:v>
       </x:c>
-      <x:c r="C52" s="1" t="s">
+      <x:c r="C52" s="2" t="s">
         <x:v>158</x:v>
       </x:c>
-      <x:c r="D52" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A53" s="1" t="s">
+      <x:c r="D52" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A53" s="2" t="s">
         <x:v>159</x:v>
       </x:c>
-      <x:c r="B53" s="1" t="s">
+      <x:c r="B53" s="2" t="s">
         <x:v>160</x:v>
       </x:c>
-      <x:c r="C53" s="1" t="s">
+      <x:c r="C53" s="2" t="s">
         <x:v>161</x:v>
       </x:c>
-      <x:c r="D53" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A54" s="1" t="s">
+      <x:c r="D53" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A54" s="2" t="s">
         <x:v>162</x:v>
       </x:c>
-      <x:c r="B54" s="1" t="s">
+      <x:c r="B54" s="2" t="s">
         <x:v>163</x:v>
       </x:c>
-      <x:c r="C54" s="1" t="s">
+      <x:c r="C54" s="2" t="s">
         <x:v>164</x:v>
       </x:c>
-      <x:c r="D54" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A55" s="1" t="s">
+      <x:c r="D54" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A55" s="2" t="s">
         <x:v>165</x:v>
       </x:c>
-      <x:c r="B55" s="1" t="s">
+      <x:c r="B55" s="2" t="s">
         <x:v>166</x:v>
       </x:c>
-      <x:c r="C55" s="1" t="s">
+      <x:c r="C55" s="2" t="s">
         <x:v>167</x:v>
       </x:c>
-      <x:c r="D55" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A56" s="1" t="s">
+      <x:c r="D55" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A56" s="2" t="s">
         <x:v>168</x:v>
       </x:c>
-      <x:c r="B56" s="1" t="s">
+      <x:c r="B56" s="2" t="s">
         <x:v>169</x:v>
       </x:c>
-      <x:c r="C56" s="1" t="s">
+      <x:c r="C56" s="2" t="s">
         <x:v>170</x:v>
       </x:c>
-      <x:c r="D56" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A57" s="1" t="s">
+      <x:c r="D56" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A57" s="2" t="s">
         <x:v>171</x:v>
       </x:c>
-      <x:c r="B57" s="1" t="s">
+      <x:c r="B57" s="2" t="s">
         <x:v>172</x:v>
       </x:c>
-      <x:c r="C57" s="1" t="s">
+      <x:c r="C57" s="2" t="s">
         <x:v>173</x:v>
       </x:c>
-      <x:c r="D57" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A58" s="1" t="s">
+      <x:c r="D57" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A58" s="2" t="s">
         <x:v>174</x:v>
       </x:c>
-      <x:c r="B58" s="1" t="s">
+      <x:c r="B58" s="2" t="s">
         <x:v>175</x:v>
       </x:c>
-      <x:c r="C58" s="1" t="s">
+      <x:c r="C58" s="2" t="s">
         <x:v>176</x:v>
       </x:c>
-      <x:c r="D58" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A59" s="1" t="s">
-        <x:v>177</x:v>
-      </x:c>
-      <x:c r="B59" s="1" t="s">
-        <x:v>178</x:v>
-      </x:c>
-      <x:c r="C59" s="1" t="s">
-        <x:v>179</x:v>
-      </x:c>
-      <x:c r="D59" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A60" s="1" t="s">
-        <x:v>180</x:v>
-      </x:c>
-      <x:c r="B60" s="1" t="s">
-        <x:v>181</x:v>
-      </x:c>
-      <x:c r="C60" s="1" t="s">
-        <x:v>182</x:v>
-      </x:c>
-      <x:c r="D60" s="1" t="s">
-        <x:v>13</x:v>
+      <x:c r="D58" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A59" s="2" t="s">
+        <x:v>174</x:v>
+      </x:c>
+      <x:c r="B59" s="2" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="C59" s="2" t="s">
+        <x:v>176</x:v>
+      </x:c>
+      <x:c r="D59" s="2" t="s">
+        <x:v>9</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2210,605 +2207,641 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E42"/>
+  <x:dimension ref="A1:F43"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="A2" sqref="A2 A2:A2"/>
+      <x:selection activeCell="F2" sqref="F2 F2:F2"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="10.561875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="21.961719" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="32.285156" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="9.85125" style="1" customWidth="1"/>
-    <x:col min="3" max="3" width="30.285156" style="1" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="9.855469" style="2" customWidth="1"/>
+    <x:col min="2" max="2" width="65.140625" style="2" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="1" t="s">
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="2" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="1" t="s">
+      <x:c r="B1" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="1" t="s">
+      <x:c r="C1" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="1" t="s">
+      <x:c r="D1" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="1" t="s">
+      <x:c r="E1" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="1" t="s">
+      <x:c r="F1" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="2" t="s">
+        <x:v>177</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>178</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s">
+        <x:v>181</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="2" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
         <x:v>183</x:v>
       </x:c>
-      <x:c r="B2" s="1" t="s">
+      <x:c r="C3" s="2" t="s">
         <x:v>184</x:v>
       </x:c>
-      <x:c r="C2" s="1" t="s">
+      <x:c r="D3" s="2" t="s">
         <x:v>185</x:v>
       </x:c>
-      <x:c r="D2" s="1" t="s">
+    </x:row>
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="2" t="s">
         <x:v>186</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="1" t="s">
+      <x:c r="B4" s="2" t="s">
         <x:v>187</x:v>
       </x:c>
-      <x:c r="B3" s="1" t="s">
+      <x:c r="C4" s="2" t="s">
         <x:v>188</x:v>
       </x:c>
-      <x:c r="C3" s="1" t="s">
+      <x:c r="D4" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
         <x:v>189</x:v>
       </x:c>
-      <x:c r="D3" s="1" t="s">
+    </x:row>
+    <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="2" t="s">
         <x:v>190</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="1" t="s">
+      <x:c r="B5" s="2" t="s">
         <x:v>191</x:v>
       </x:c>
-      <x:c r="B4" s="1" t="s">
+      <x:c r="C5" s="2" t="s">
         <x:v>192</x:v>
       </x:c>
-      <x:c r="C4" s="1" t="s">
+      <x:c r="D5" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="2" t="s">
         <x:v>193</x:v>
       </x:c>
-      <x:c r="D4" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="1" t="s">
+      <x:c r="B6" s="2" t="s">
         <x:v>194</x:v>
       </x:c>
-      <x:c r="B5" s="1" t="s">
+      <x:c r="C6" s="2" t="s">
         <x:v>195</x:v>
       </x:c>
-      <x:c r="C5" s="1" t="s">
+      <x:c r="D6" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="2" t="s">
         <x:v>196</x:v>
       </x:c>
-      <x:c r="D5" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="1" t="s">
+      <x:c r="B7" s="2" t="s">
         <x:v>197</x:v>
       </x:c>
-      <x:c r="B6" s="1" t="s">
+      <x:c r="C7" s="2" t="s">
         <x:v>198</x:v>
       </x:c>
-      <x:c r="C6" s="1" t="s">
+      <x:c r="D7" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="2" t="s">
         <x:v>199</x:v>
       </x:c>
-      <x:c r="D6" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="1" t="s">
+      <x:c r="B8" s="2" t="s">
         <x:v>200</x:v>
       </x:c>
-      <x:c r="B7" s="1" t="s">
+      <x:c r="C8" s="2" t="s">
         <x:v>201</x:v>
       </x:c>
-      <x:c r="C7" s="1" t="s">
+      <x:c r="D8" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="2" t="s">
         <x:v>202</x:v>
       </x:c>
-      <x:c r="D7" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="1" t="s">
+      <x:c r="B9" s="2" t="s">
         <x:v>203</x:v>
       </x:c>
-      <x:c r="B8" s="1" t="s">
+      <x:c r="C9" s="2" t="s">
         <x:v>204</x:v>
       </x:c>
-      <x:c r="C8" s="1" t="s">
+      <x:c r="D9" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="2" t="s">
         <x:v>205</x:v>
       </x:c>
-      <x:c r="D8" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="1" t="s">
+      <x:c r="B10" s="2" t="s">
         <x:v>206</x:v>
       </x:c>
-      <x:c r="B9" s="1" t="s">
+      <x:c r="C10" s="2" t="s">
         <x:v>207</x:v>
       </x:c>
-      <x:c r="C9" s="1" t="s">
+      <x:c r="D10" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="2" t="s">
         <x:v>208</x:v>
       </x:c>
-      <x:c r="D9" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="1" t="s">
+      <x:c r="B11" s="2" t="s">
         <x:v>209</x:v>
       </x:c>
-      <x:c r="B10" s="1" t="s">
+      <x:c r="C11" s="2" t="s">
         <x:v>210</x:v>
       </x:c>
-      <x:c r="C10" s="1" t="s">
+      <x:c r="D11" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="2" t="s">
         <x:v>211</x:v>
       </x:c>
-      <x:c r="D10" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="1" t="s">
+      <x:c r="B12" s="2" t="s">
         <x:v>212</x:v>
       </x:c>
-      <x:c r="B11" s="1" t="s">
+      <x:c r="C12" s="2" t="s">
         <x:v>213</x:v>
       </x:c>
-      <x:c r="C11" s="1" t="s">
+      <x:c r="D12" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="2" t="s">
         <x:v>214</x:v>
       </x:c>
-      <x:c r="D11" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="1" t="s">
+      <x:c r="B13" s="2" t="s">
         <x:v>215</x:v>
       </x:c>
-      <x:c r="B12" s="1" t="s">
+      <x:c r="C13" s="2" t="s">
         <x:v>216</x:v>
       </x:c>
-      <x:c r="C12" s="1" t="s">
+      <x:c r="D13" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="2" t="s">
         <x:v>217</x:v>
       </x:c>
-      <x:c r="D12" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A13" s="1" t="s">
+      <x:c r="B14" s="2" t="s">
         <x:v>218</x:v>
       </x:c>
-      <x:c r="B13" s="1" t="s">
+      <x:c r="C14" s="2" t="s">
         <x:v>219</x:v>
       </x:c>
-      <x:c r="C13" s="1" t="s">
+      <x:c r="D14" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="2" t="s">
         <x:v>220</x:v>
       </x:c>
-      <x:c r="D13" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A14" s="1" t="s">
+      <x:c r="B15" s="2" t="s">
         <x:v>221</x:v>
       </x:c>
-      <x:c r="B14" s="1" t="s">
+      <x:c r="C15" s="2" t="s">
         <x:v>222</x:v>
       </x:c>
-      <x:c r="C14" s="1" t="s">
+      <x:c r="D15" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A16" s="2" t="s">
         <x:v>223</x:v>
       </x:c>
-      <x:c r="D14" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A15" s="1" t="s">
+      <x:c r="B16" s="2" t="s">
         <x:v>224</x:v>
       </x:c>
-      <x:c r="B15" s="1" t="s">
+      <x:c r="C16" s="2" t="s">
         <x:v>225</x:v>
       </x:c>
-      <x:c r="C15" s="1" t="s">
+      <x:c r="D16" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A17" s="2" t="s">
         <x:v>226</x:v>
       </x:c>
-      <x:c r="D15" s="1" t="s">
-        <x:v>190</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A16" s="1" t="s">
+      <x:c r="B17" s="2" t="s">
         <x:v>227</x:v>
       </x:c>
-      <x:c r="B16" s="1" t="s">
+      <x:c r="C17" s="2" t="s">
         <x:v>228</x:v>
       </x:c>
-      <x:c r="C16" s="1" t="s">
+      <x:c r="D17" s="2" t="s">
+        <x:v>185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A18" s="2" t="s">
         <x:v>229</x:v>
       </x:c>
-      <x:c r="D16" s="1" t="s">
+      <x:c r="B18" s="2" t="s">
         <x:v>230</x:v>
       </x:c>
-    </x:row>
-    <x:row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A17" s="1" t="s">
+      <x:c r="C18" s="2" t="s">
         <x:v>231</x:v>
       </x:c>
-      <x:c r="B17" s="1" t="s">
+      <x:c r="D18" s="2" t="s">
         <x:v>232</x:v>
       </x:c>
-      <x:c r="C17" s="1" t="s">
+    </x:row>
+    <x:row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A19" s="2" t="s">
         <x:v>233</x:v>
       </x:c>
-      <x:c r="D17" s="1" t="s">
-        <x:v>230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A18" s="1" t="s">
+      <x:c r="B19" s="2" t="s">
         <x:v>234</x:v>
       </x:c>
-      <x:c r="B18" s="1" t="s">
+      <x:c r="C19" s="2" t="s">
         <x:v>235</x:v>
       </x:c>
-      <x:c r="C18" s="1" t="s">
+      <x:c r="D19" s="2" t="s">
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A20" s="2" t="s">
         <x:v>236</x:v>
       </x:c>
-      <x:c r="D18" s="1" t="s">
-        <x:v>230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A19" s="1" t="s">
+      <x:c r="B20" s="2" t="s">
         <x:v>237</x:v>
       </x:c>
-      <x:c r="B19" s="1" t="s">
+      <x:c r="C20" s="2" t="s">
         <x:v>238</x:v>
       </x:c>
-      <x:c r="C19" s="1" t="s">
+      <x:c r="D20" s="2" t="s">
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A21" s="2" t="s">
         <x:v>239</x:v>
       </x:c>
-      <x:c r="D19" s="1" t="s">
-        <x:v>230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A20" s="1" t="s">
+      <x:c r="B21" s="2" t="s">
         <x:v>240</x:v>
       </x:c>
-      <x:c r="B20" s="1" t="s">
+      <x:c r="C21" s="2" t="s">
         <x:v>241</x:v>
       </x:c>
-      <x:c r="C20" s="1" t="s">
+      <x:c r="D21" s="2" t="s">
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A22" s="2" t="s">
         <x:v>242</x:v>
       </x:c>
-      <x:c r="D20" s="1" t="s">
-        <x:v>230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A21" s="1" t="s">
+      <x:c r="B22" s="2" t="s">
         <x:v>243</x:v>
       </x:c>
-      <x:c r="B21" s="1" t="s">
+      <x:c r="C22" s="2" t="s">
         <x:v>244</x:v>
       </x:c>
-      <x:c r="C21" s="1" t="s">
+      <x:c r="D22" s="2" t="s">
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A23" s="2" t="s">
         <x:v>245</x:v>
       </x:c>
-      <x:c r="D21" s="1" t="s">
-        <x:v>230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A22" s="1" t="s">
+      <x:c r="B23" s="2" t="s">
         <x:v>246</x:v>
       </x:c>
-      <x:c r="B22" s="1" t="s">
+      <x:c r="C23" s="2" t="s">
         <x:v>247</x:v>
       </x:c>
-      <x:c r="C22" s="1" t="s">
+      <x:c r="D23" s="2" t="s">
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A24" s="2" t="s">
         <x:v>248</x:v>
       </x:c>
-      <x:c r="D22" s="1" t="s">
-        <x:v>230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A23" s="1" t="s">
+      <x:c r="B24" s="2" t="s">
         <x:v>249</x:v>
       </x:c>
-      <x:c r="B23" s="1" t="s">
+      <x:c r="C24" s="2" t="s">
         <x:v>250</x:v>
       </x:c>
-      <x:c r="C23" s="1" t="s">
+      <x:c r="D24" s="2" t="s">
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A25" s="2" t="s">
         <x:v>251</x:v>
       </x:c>
-      <x:c r="D23" s="1" t="s">
-        <x:v>230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A24" s="1" t="s">
+      <x:c r="B25" s="2" t="s">
         <x:v>252</x:v>
       </x:c>
-      <x:c r="B24" s="1" t="s">
+      <x:c r="C25" s="2" t="s">
         <x:v>253</x:v>
       </x:c>
-      <x:c r="C24" s="1" t="s">
+      <x:c r="D25" s="2" t="s">
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A26" s="2" t="s">
         <x:v>254</x:v>
       </x:c>
-      <x:c r="D24" s="1" t="s">
-        <x:v>230</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A25" s="1" t="s">
+      <x:c r="B26" s="2" t="s">
         <x:v>255</x:v>
       </x:c>
-      <x:c r="B25" s="1" t="s">
+      <x:c r="C26" s="2" t="s">
         <x:v>256</x:v>
       </x:c>
-      <x:c r="C25" s="1" t="s">
+      <x:c r="D26" s="2" t="s">
+        <x:v>232</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A27" s="2" t="s">
         <x:v>257</x:v>
       </x:c>
-      <x:c r="D25" s="1" t="s">
+      <x:c r="B27" s="2" t="s">
         <x:v>258</x:v>
       </x:c>
-    </x:row>
-    <x:row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A26" s="1" t="s">
+      <x:c r="C27" s="2" t="s">
         <x:v>259</x:v>
       </x:c>
-      <x:c r="B26" s="1" t="s">
+      <x:c r="D27" s="2" t="s">
         <x:v>260</x:v>
       </x:c>
-      <x:c r="C26" s="1" t="s">
+    </x:row>
+    <x:row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A28" s="2" t="s">
         <x:v>261</x:v>
       </x:c>
-      <x:c r="D26" s="1" t="s">
-        <x:v>258</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A27" s="1" t="s">
+      <x:c r="B28" s="2" t="s">
         <x:v>262</x:v>
       </x:c>
-      <x:c r="B27" s="1" t="s">
+      <x:c r="C28" s="2" t="s">
         <x:v>263</x:v>
       </x:c>
-      <x:c r="C27" s="1" t="s">
+      <x:c r="D28" s="2" t="s">
+        <x:v>260</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A29" s="2" t="s">
         <x:v>264</x:v>
       </x:c>
-      <x:c r="D27" s="1" t="s">
-        <x:v>258</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A28" s="1" t="s">
+      <x:c r="B29" s="2" t="s">
         <x:v>265</x:v>
       </x:c>
-      <x:c r="B28" s="1" t="s">
+      <x:c r="C29" s="2" t="s">
         <x:v>266</x:v>
       </x:c>
-      <x:c r="C28" s="1" t="s">
+      <x:c r="D29" s="2" t="s">
+        <x:v>260</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A30" s="2" t="s">
         <x:v>267</x:v>
       </x:c>
-      <x:c r="D28" s="1" t="s">
-        <x:v>258</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A29" s="1" t="s">
+      <x:c r="B30" s="2" t="s">
         <x:v>268</x:v>
       </x:c>
-      <x:c r="B29" s="1" t="s">
+      <x:c r="C30" s="2" t="s">
         <x:v>269</x:v>
       </x:c>
-      <x:c r="C29" s="1" t="s">
+      <x:c r="D30" s="2" t="s">
+        <x:v>260</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A31" s="2" t="s">
         <x:v>270</x:v>
       </x:c>
-      <x:c r="D29" s="1" t="s">
-        <x:v>258</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A30" s="1" t="s">
+      <x:c r="B31" s="2" t="s">
         <x:v>271</x:v>
       </x:c>
-      <x:c r="B30" s="1" t="s">
+      <x:c r="C31" s="2" t="s">
         <x:v>272</x:v>
       </x:c>
-      <x:c r="C30" s="1" t="s">
+      <x:c r="D31" s="2" t="s">
+        <x:v>260</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A32" s="2" t="s">
         <x:v>273</x:v>
       </x:c>
-      <x:c r="D30" s="1" t="s">
-        <x:v>258</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A31" s="1" t="s">
+      <x:c r="B32" s="2" t="s">
         <x:v>274</x:v>
       </x:c>
-      <x:c r="B31" s="1" t="s">
+      <x:c r="C32" s="2" t="s">
         <x:v>275</x:v>
       </x:c>
-      <x:c r="C31" s="1" t="s">
+      <x:c r="D32" s="2" t="s">
+        <x:v>260</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A33" s="2" t="s">
         <x:v>276</x:v>
       </x:c>
-      <x:c r="D31" s="1" t="s">
-        <x:v>258</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A32" s="1" t="s">
+      <x:c r="B33" s="2" t="s">
         <x:v>277</x:v>
       </x:c>
-      <x:c r="B32" s="1" t="s">
+      <x:c r="C33" s="2" t="s">
         <x:v>278</x:v>
       </x:c>
-      <x:c r="C32" s="1" t="s">
+      <x:c r="D33" s="2" t="s">
+        <x:v>260</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A34" s="2" t="s">
         <x:v>279</x:v>
       </x:c>
-      <x:c r="D32" s="1" t="s">
+      <x:c r="B34" s="2" t="s">
         <x:v>280</x:v>
       </x:c>
-    </x:row>
-    <x:row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A33" s="1" t="s">
+      <x:c r="C34" s="2" t="s">
         <x:v>281</x:v>
       </x:c>
-      <x:c r="B33" s="1" t="s">
+      <x:c r="D34" s="2" t="s">
         <x:v>282</x:v>
       </x:c>
-      <x:c r="C33" s="1" t="s">
+    </x:row>
+    <x:row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A35" s="2" t="s">
         <x:v>283</x:v>
       </x:c>
-      <x:c r="D33" s="1" t="s">
-        <x:v>280</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A34" s="1" t="s">
-        <x:v>106</x:v>
-      </x:c>
-      <x:c r="B34" s="1" t="s">
+      <x:c r="B35" s="2" t="s">
         <x:v>284</x:v>
       </x:c>
-      <x:c r="C34" s="1" t="s">
+      <x:c r="C35" s="2" t="s">
         <x:v>285</x:v>
       </x:c>
-      <x:c r="D34" s="1" t="s">
-        <x:v>280</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A35" s="1" t="s">
+      <x:c r="D35" s="2" t="s">
+        <x:v>282</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A36" s="2" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B36" s="2" t="s">
         <x:v>286</x:v>
       </x:c>
-      <x:c r="B35" s="1" t="s">
+      <x:c r="C36" s="2" t="s">
         <x:v>287</x:v>
       </x:c>
-      <x:c r="C35" s="1" t="s">
+      <x:c r="D36" s="2" t="s">
+        <x:v>282</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A37" s="2" t="s">
         <x:v>288</x:v>
       </x:c>
-      <x:c r="D35" s="1" t="s">
-        <x:v>280</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A36" s="1" t="s">
+      <x:c r="B37" s="2" t="s">
         <x:v>289</x:v>
       </x:c>
-      <x:c r="B36" s="1" t="s">
+      <x:c r="C37" s="2" t="s">
         <x:v>290</x:v>
       </x:c>
-      <x:c r="C36" s="1" t="s">
+      <x:c r="D37" s="2" t="s">
+        <x:v>282</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A38" s="2" t="s">
         <x:v>291</x:v>
       </x:c>
-      <x:c r="D36" s="1" t="s">
+      <x:c r="B38" s="2" t="s">
         <x:v>292</x:v>
       </x:c>
-    </x:row>
-    <x:row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A37" s="1" t="s">
+      <x:c r="C38" s="2" t="s">
         <x:v>293</x:v>
       </x:c>
-      <x:c r="B37" s="1" t="s">
+      <x:c r="D38" s="2" t="s">
         <x:v>294</x:v>
       </x:c>
-      <x:c r="C37" s="1" t="s">
+    </x:row>
+    <x:row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A39" s="2" t="s">
         <x:v>295</x:v>
       </x:c>
-      <x:c r="D37" s="1" t="s">
+      <x:c r="B39" s="2" t="s">
         <x:v>296</x:v>
       </x:c>
-    </x:row>
-    <x:row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A38" s="1" t="s">
+      <x:c r="C39" s="2" t="s">
         <x:v>297</x:v>
       </x:c>
-      <x:c r="B38" s="1" t="s">
+      <x:c r="D39" s="2" t="s">
         <x:v>298</x:v>
       </x:c>
-      <x:c r="C38" s="1" t="s">
+    </x:row>
+    <x:row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A40" s="2" t="s">
         <x:v>299</x:v>
       </x:c>
-      <x:c r="D38" s="1" t="s">
+      <x:c r="B40" s="2" t="s">
         <x:v>300</x:v>
       </x:c>
-    </x:row>
-    <x:row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A39" s="1" t="s">
+      <x:c r="C40" s="2" t="s">
         <x:v>301</x:v>
       </x:c>
-      <x:c r="C39" s="1" t="s">
+      <x:c r="D40" s="2" t="s">
         <x:v>302</x:v>
       </x:c>
-      <x:c r="D39" s="1" t="s">
-        <x:v>300</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A40" s="1" t="s">
+    </x:row>
+    <x:row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A41" s="2" t="s">
         <x:v>303</x:v>
       </x:c>
-      <x:c r="B40" s="1" t="s">
+      <x:c r="C41" s="2" t="s">
         <x:v>304</x:v>
       </x:c>
-      <x:c r="C40" s="1" t="s">
+      <x:c r="D41" s="2" t="s">
+        <x:v>302</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A42" s="2" t="s">
         <x:v>305</x:v>
       </x:c>
-      <x:c r="D40" s="1" t="s">
-        <x:v>300</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A41" s="1" t="s">
+      <x:c r="B42" s="2" t="s">
         <x:v>306</x:v>
       </x:c>
-      <x:c r="B41" s="1" t="s">
+      <x:c r="C42" s="2" t="s">
         <x:v>307</x:v>
       </x:c>
-      <x:c r="C41" s="1" t="s">
+      <x:c r="D42" s="2" t="s">
+        <x:v>302</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <x:c r="A43" s="2" t="s">
         <x:v>308</x:v>
       </x:c>
-      <x:c r="D41" s="1" t="s">
+      <x:c r="B43" s="2" t="s">
         <x:v>309</x:v>
       </x:c>
-    </x:row>
-    <x:row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A42" s="1" t="s">
+      <x:c r="C43" s="2" t="s">
         <x:v>310</x:v>
       </x:c>
-      <x:c r="B42" s="1" t="s">
+      <x:c r="D43" s="2" t="s">
         <x:v>311</x:v>
       </x:c>
-      <x:c r="C42" s="1" t="s">
+    </x:row>
+    <x:row r="44" spans="1:6">
+      <x:c r="A44" s="2" t="s">
         <x:v>312</x:v>
       </x:c>
-      <x:c r="D42" s="1" t="s">
-        <x:v>309</x:v>
+      <x:c r="B44" s="2" t="s">
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="C44" s="2" t="s">
+        <x:v>314</x:v>
+      </x:c>
+      <x:c r="D44" s="2" t="s">
+        <x:v>311</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Optimización de control de errores. Mejoras en el sistema de formato final del reporte.
</commit_message>
<xml_diff>
--- a/Archivos/Comentarios.xlsx
+++ b/Archivos/Comentarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_0DDAEE711ED83A34E52B4628AADB90D7BD4B3E81" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{20655533-1558-4B7B-A1FA-3D6E302A1C9B}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_CFCB90BAC2EDAA75E4866A1AB923BEB7F2D0FA3F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4C404A26-7062-48FB-A1AE-B6FB3A2D8314}"/>
   <bookViews>
-    <workbookView xWindow="30270" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nuevos" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <author>Jorge Alejandro Falcon Alvarez</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{55BE28E5-52EB-4E59-BDA8-E4E22EFEBFB0}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C3ABF732-BC3B-41EA-B564-3A23AF6F7296}">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{F2485DEA-31C0-4E8E-9B54-824E509BB300}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2F3809BF-0A8A-4B77-94C7-B08AC4A32CBD}">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{8AEC648A-819D-4BC3-8006-2C40145D86AE}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{9475D162-46C8-44BE-9B58-73474C11F41C}">
       <text>
         <r>
           <rPr>
@@ -68,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{7DE0D5D9-4259-4007-9801-3DA2ED58F74A}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{CCC3E864-2F0F-4E85-B8C0-50366E5ED399}">
       <text>
         <r>
           <rPr>
@@ -82,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{36EAF185-7DED-4AA5-8527-F466E51EE244}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{364C5A4C-3FE5-41D4-946D-C9F823438EE3}">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{966EAA59-AF8B-4160-9F92-36AD0F740A8B}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{ECFC2985-4CE6-4332-87CB-604EAA680A7B}">
       <text>
         <r>
           <rPr>
@@ -110,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{96499CC4-84D0-40D4-85F1-CB4E8D08C82B}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{83C26998-0BA1-43A6-9BC0-E7923F131448}">
       <text>
         <r>
           <rPr>
@@ -134,7 +134,7 @@
     <author>Jorge Alejandro Falcon Alvarez</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B05FA9D9-4952-4C63-B463-04E2C7D2B06B}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{9C6EFED4-31E9-4B8D-A5E1-8E28C98C193F}">
       <text>
         <r>
           <rPr>
@@ -148,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5E7C1575-46C0-419A-91A5-42E5BFC8E24A}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5490D3F2-40C6-4216-A4A7-BFD47AF70A0D}">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{239BBC01-7969-4B73-8296-DDC97E078C52}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{EE10647F-9824-472D-A560-5A03A34BF99C}">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{E193FABA-B5B0-46AF-A0DE-8E2FF9665246}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{F535E96F-B674-40AC-854A-DF3105A42478}">
       <text>
         <r>
           <rPr>
@@ -190,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{A062C6F2-EC43-4B77-A2D5-09D8FC7367C3}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{3209D7C8-0BCF-46F1-977A-E9E730FB8DC4}">
       <text>
         <r>
           <rPr>
@@ -204,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{3D2469D7-324A-4FDA-9159-696624DA33E3}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{9E16ADE9-F8AB-4718-8B58-86AC88825BCD}">
       <text>
         <r>
           <rPr>
@@ -218,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{3D73DBF6-54AE-4E4D-835B-478085B388DB}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{30055440-F319-4561-A564-0ADEE680BA63}">
       <text>
         <r>
           <rPr>
@@ -237,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="84">
   <si>
     <t>Nombre</t>
   </si>
@@ -269,137 +269,119 @@
     <t>Respuestas</t>
   </si>
   <si>
-    <t>eduardog89</t>
-  </si>
-  <si>
-    <t>espero mucho de este curso! me gustaria ser un especialisa en RPA</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408059/</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>Jorge Alejandro Falcon Alvarez</t>
+  </si>
+  <si>
+    <t>Posterior a la creación de la carpeta, debemos dar clic derecho sobre la carpeta, luego en Add y seleccionamos "Sequence" para crear el XAML. Otra forma de crear el XAML es dar clic derecho sobre la Sequence que tenemos en nuestro Main, luego elegimos "Extract as Workflow"</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408928/</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>Curso de Automatización de Procesos RPA con UiPath</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>me salen dos versiones… studio y studio X…una es la version de paga o algo asi?</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408105/</t>
-  </si>
-  <si>
-    <t>vamonos!</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408102/</t>
-  </si>
-  <si>
-    <t>todo listo hasta ahora…</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408159/</t>
-  </si>
-  <si>
-    <t>Así esta bien? me imagino que todavia no se sube todo el curso cierto? pero si este es el temario suena genial</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408207/</t>
-  </si>
-  <si>
-    <t>miniendo</t>
-  </si>
-  <si>
-    <t>Actualmente trabajo como Tester he tenido algo de contacto con procesos automatizados estoy anciancioso por aprender mas de procesos de automatizacio con esta herramienta y mejorar mi perfil profesional.</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406921/</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
-    <t>Andres Felipe Bravo Piñeros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Super!!! Trabajo con RPA a través de la herramienta Automation Anywhere pero estoy ansioso de aprender y empezar a trabajar con UiPath </t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406612/</t>
-  </si>
-  <si>
-    <t>Lisa Daniela Villar Contreras</t>
-  </si>
-  <si>
-    <t>Esperaba mucho este curso ! Gracias</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406518/</t>
-  </si>
-  <si>
-    <t>Víctor León</t>
-  </si>
-  <si>
-    <t>Esperaba este curso</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406307/</t>
-  </si>
-  <si>
-    <t>Gonzalo Flores</t>
-  </si>
-  <si>
-    <t>Excelente, empezamos con toda la actitud</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406228/</t>
-  </si>
-  <si>
-    <t>German_Danilo_Forero</t>
-  </si>
-  <si>
-    <t>Explicación clara y prática, empezamos bien.</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406118/</t>
-  </si>
-  <si>
-    <t>Brayan Potosi Dominguez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Que introducción tan innovadora </t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406091/</t>
-  </si>
-  <si>
-    <t>Nicolas Antognoli</t>
-  </si>
-  <si>
-    <t>Actualmente donde trabajo usamos UIPath para la carga de facturas de proveedores y funciona perfecto el OCR leyendo las mismas. Y cuando algún dato no encuentra pregunta por mail para continuar con la carga. Tambien para cargar datos de tipo de cambio a los sistemas, conciliaciones bancarias, etc.etc… Yo creo que lo mejor es comenzar con procesos chicos, y luego ir agarrando impulso con proyectos mas grandes, para que entiendan el potencial de la herramienta. El miedo al reemplazo a veces genera que no se abran para estas tecnologías, pero en realidad tienen que convivir ambas, y donde se generan procesos repetitivos dar lugar al RPA para que las personas se enfoquen mas en temas de análisis.</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406404/</t>
-  </si>
-  <si>
-    <t>yeisonmmartinez</t>
-  </si>
-  <si>
-    <t>Sería bueno conocer cuáles artefactos genera cada rol para darle claridad a su aporte en el proceso</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1407719/</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>eduardog89</t>
+  </si>
+  <si>
+    <t>espero mucho de este curso! me gustaria ser un especialisa en RPA</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408059/</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
+    <t>Contiene respuestas demasiado largas para ser soportadas en esta versión.</t>
+  </si>
+  <si>
+    <t>miniendo</t>
+  </si>
+  <si>
+    <t>Actualmente trabajo como Tester he tenido algo de contacto con procesos automatizados estoy anciancioso por aprender mas de procesos de automatizacio con esta herramienta y mejorar mi perfil profesional.</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406921/</t>
+  </si>
+  <si>
+    <t>Andres Felipe Bravo Piñeros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super!!! Trabajo con RPA a través de la herramienta Automation Anywhere pero estoy ansioso de aprender y empezar a trabajar con UiPath </t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406612/</t>
+  </si>
+  <si>
+    <t>Lisa Daniela Villar Contreras</t>
+  </si>
+  <si>
+    <t>Esperaba mucho este curso ! Gracias</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406518/</t>
+  </si>
+  <si>
+    <t>Víctor León</t>
+  </si>
+  <si>
+    <t>Esperaba este curso</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406307/</t>
+  </si>
+  <si>
+    <t>Gonzalo Flores</t>
+  </si>
+  <si>
+    <t>Excelente, empezamos con toda la actitud</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406228/</t>
+  </si>
+  <si>
+    <t>German_Danilo_Forero</t>
+  </si>
+  <si>
+    <t>Explicación clara y prática, empezamos bien.</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406118/</t>
+  </si>
+  <si>
+    <t>Brayan Potosi Dominguez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que introducción tan innovadora </t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406091/</t>
+  </si>
+  <si>
+    <t>yeisonmmartinez</t>
+  </si>
+  <si>
+    <t>Sería bueno conocer cuáles artefactos genera cada rol para darle claridad a su aporte en el proceso</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1407719/</t>
+  </si>
+  <si>
     <t>jfespanolito : Gracias por la recomendación, revisaré como integrarlo en esta clase.</t>
   </si>
   <si>
@@ -428,6 +410,18 @@
     <t>platzi.com/comentario/1406132/</t>
   </si>
   <si>
+    <t>me salen dos versiones… studio y studio X…una es la version de paga o algo asi?</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408105/</t>
+  </si>
+  <si>
+    <t>vamonos!</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408102/</t>
+  </si>
+  <si>
     <t>En el siguiente enlace pueden verificar los requerimientos de Hardware y Software recomendados</t>
   </si>
   <si>
@@ -446,6 +440,27 @@
     <t>platzi.com/comentario/1406138/</t>
   </si>
   <si>
+    <t>Carlos Abel Dominguez Bautista</t>
+  </si>
+  <si>
+    <t>Brutal!</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408798/</t>
+  </si>
+  <si>
+    <t>todo listo hasta ahora…</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408159/</t>
+  </si>
+  <si>
+    <t>Con la versión community cómo se realiza el despliegue de un robot en producción?</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1407814/</t>
+  </si>
+  <si>
     <t>Marcelo Ganin</t>
   </si>
   <si>
@@ -455,10 +470,28 @@
     <t>platzi.com/comentario/1406205/</t>
   </si>
   <si>
-    <t>Con la versión community cómo se realiza el despliegue de un robot en producción?</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1407814/</t>
+    <t>Así esta bien? me imagino que todavia no se sube todo el curso cierto? pero si este es el temario suena genial</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408207/</t>
+  </si>
+  <si>
+    <t>no se me creo automaticamente el archio EscribirHolaMundo.xaml … apesar que al ejecutar el robot si se ejecuto bien… tuve que realizarlo manualmente…porque a ti se te creo automaticamente el “XAML de Hola mundo” ?</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408315/</t>
+  </si>
+  <si>
+    <t>Nicolas Antognoli</t>
+  </si>
+  <si>
+    <t>Actualmente donde trabajo usamos UIPath para la carga de facturas de proveedores y funciona perfecto el OCR leyendo las mismas. Y cuando algún dato no encuentra pregunta por mail para continuar con la carga. Tambien para cargar datos de tipo de cambio a los sistemas, conciliaciones bancarias, etc.etc… Yo creo que lo mejor es comenzar con procesos chicos, y luego ir agarrando impulso con proyectos mas grandes, para que entiendan el potencial de la herramienta. El miedo al reemplazo a veces genera que no se abran para estas tecnologías, pero en realidad tienen que convivir ambas, y donde se generan procesos repetitivos dar lugar al RPA para que las personas se enfoquen mas en temas de análisis.</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406404/</t>
+  </si>
+  <si>
+    <t>jfespanolito : Así es, hay que convivir y crecer poco a poco… Gran recomendación, gracias por ella.</t>
   </si>
 </sst>
 </file>
@@ -500,10 +533,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,34 +843,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
-    <col min="3" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="50.7109375" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" style="1" bestFit="1" customWidth="1"/>
@@ -894,8 +911,11 @@
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -903,10 +923,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -914,602 +934,762 @@
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J37" sqref="J2:J37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="G6" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>69</v>
@@ -1518,85 +1698,199 @@
         <v>70</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrección de URL de navegación a Respuestas.
</commit_message>
<xml_diff>
--- a/Archivos/Comentarios.xlsx
+++ b/Archivos/Comentarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_CFCB90BAC2EDAA75E4866A1AB923BEB7F2D0FA3F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4C404A26-7062-48FB-A1AE-B6FB3A2D8314}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="11_7B0B509AF2B52B0BCE3AA4C74557EF70EEF2F657" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87D42317-A5BB-4C51-801F-5B264EA0617D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30270" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nuevos" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <author>Jorge Alejandro Falcon Alvarez</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C3ABF732-BC3B-41EA-B564-3A23AF6F7296}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{35CB721E-BFD1-4F36-BE1C-981506CC0C65}">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2F3809BF-0A8A-4B77-94C7-B08AC4A32CBD}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6FDF43BB-3244-43AD-8C9D-9C739EFB7DE5}">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{9475D162-46C8-44BE-9B58-73474C11F41C}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1D7C3363-A5DA-46CE-91DD-8EC004C662C7}">
       <text>
         <r>
           <rPr>
@@ -68,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{CCC3E864-2F0F-4E85-B8C0-50366E5ED399}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{7DD63EB1-A5C4-4504-91E7-16A6B6DB7D18}">
       <text>
         <r>
           <rPr>
@@ -82,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{364C5A4C-3FE5-41D4-946D-C9F823438EE3}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{3384876E-CA5F-4C2C-821B-9110DF0F1381}">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{ECFC2985-4CE6-4332-87CB-604EAA680A7B}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{C5305301-4922-46DD-BAD6-A5EE5AA03A46}">
       <text>
         <r>
           <rPr>
@@ -110,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{83C26998-0BA1-43A6-9BC0-E7923F131448}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{DAF851A3-DCE5-4FE5-93AD-77EDC601DF51}">
       <text>
         <r>
           <rPr>
@@ -134,7 +134,7 @@
     <author>Jorge Alejandro Falcon Alvarez</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{9C6EFED4-31E9-4B8D-A5E1-8E28C98C193F}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{2A005B76-DA71-4550-87CB-33BD2F383206}">
       <text>
         <r>
           <rPr>
@@ -148,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5490D3F2-40C6-4216-A4A7-BFD47AF70A0D}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{3C1BA7BC-BE40-4919-8866-914244E7777C}">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{EE10647F-9824-472D-A560-5A03A34BF99C}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{B3ADD2FF-76EE-4BCD-84B7-19353002DA1E}">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{F535E96F-B674-40AC-854A-DF3105A42478}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{151A7C4F-297D-4D4C-B0CA-616F2D52662C}">
       <text>
         <r>
           <rPr>
@@ -190,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{3209D7C8-0BCF-46F1-977A-E9E730FB8DC4}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{89976F48-A6D8-4E41-94DF-5F19A2824F62}">
       <text>
         <r>
           <rPr>
@@ -204,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{9E16ADE9-F8AB-4718-8B58-86AC88825BCD}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{CEEBCCD0-3763-461B-8DAE-15FDB5125F19}">
       <text>
         <r>
           <rPr>
@@ -218,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{30055440-F319-4561-A564-0ADEE680BA63}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{F033482E-2640-439E-A30F-1C221C80C916}">
       <text>
         <r>
           <rPr>
@@ -237,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="92">
   <si>
     <t>Nombre</t>
   </si>
@@ -269,6 +269,24 @@
     <t>Respuestas</t>
   </si>
   <si>
+    <t>Alvaro Fernández Ochoa</t>
+  </si>
+  <si>
+    <t>El error es que tiene el mismo nombre el archivo supongo.</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1409472/</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Curso de Automatización de Procesos RPA con UiPath</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>Jorge Alejandro Falcon Alvarez</t>
   </si>
   <si>
@@ -276,19 +294,26 @@
   </si>
   <si>
     <t>platzi.com/comentario/1408928/</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Curso de Automatización de Procesos RPA con UiPath</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
-    <t>0</t>
+    <t>victor rodriguez</t>
+  </si>
+  <si>
+    <t>Profe Jorge.
+¿A que se refiere con enfocar la aplicación?</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1409318/</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Contiene respuestas demasiado largas para ser soportadas en esta versión.</t>
   </si>
   <si>
     <t>eduardog89</t>
@@ -298,18 +323,12 @@
   </si>
   <si>
     <t>platzi.com/comentario/1408059/</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
-    <t>Contiene respuestas demasiado largas para ser soportadas en esta versión.</t>
-  </si>
-  <si>
     <t>miniendo</t>
   </si>
   <si>
@@ -326,6 +345,9 @@
   </si>
   <si>
     <t>platzi.com/comentario/1406612/</t>
+  </si>
+  <si>
+    <t>jfespanolito : Welcome to the dark side.jpg</t>
   </si>
   <si>
     <t>Lisa Daniela Villar Contreras</t>
@@ -489,6 +511,10 @@
   </si>
   <si>
     <t>platzi.com/comentario/1406404/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
   </si>
   <si>
     <t>jfespanolito : Así es, hay que convivir y crecer poco a poco… Gran recomendación, gracias por ella.</t>
@@ -536,10 +562,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="justify"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,11 +869,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -864,38 +888,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -911,14 +935,11 @@
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -934,11 +955,54 @@
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -949,11 +1013,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J2:J37"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -962,7 +1024,7 @@
     <col min="3" max="3" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -970,112 +1032,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -1086,20 +1146,19 @@
         <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -1110,166 +1169,163 @@
         <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1280,20 +1336,19 @@
         <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1304,118 +1359,114 @@
         <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
@@ -1426,20 +1477,19 @@
         <v>50</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
@@ -1450,447 +1500,463 @@
         <v>53</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="B33" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>83</v>
+        <v>15</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ahora se solicita la ruta donde se guardará el archivo. Se añade validación contra "navegación a url de tipo "cursos" en vez de "clases"
</commit_message>
<xml_diff>
--- a/Archivos/Comentarios.xlsx
+++ b/Archivos/Comentarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_7B0B509AF2B52B0BCE3AA4C74557EF70EEF2F657" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87D42317-A5BB-4C51-801F-5B264EA0617D}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="11_3073F1A66CECAA25EA8A224031E1565DDEC81B98" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{24576135-35A4-442F-A378-720D5F1D161B}"/>
   <bookViews>
-    <workbookView xWindow="30270" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30975" yWindow="1380" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nuevos" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <author>Jorge Alejandro Falcon Alvarez</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{35CB721E-BFD1-4F36-BE1C-981506CC0C65}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{4658A65F-C538-4F06-813B-F4B39DF2C7A3}">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6FDF43BB-3244-43AD-8C9D-9C739EFB7DE5}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{3253681F-4806-4A72-982F-3B8E314D87A8}">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1D7C3363-A5DA-46CE-91DD-8EC004C662C7}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{814A1CC0-BEC1-4CA0-8E33-452FB41321C3}">
       <text>
         <r>
           <rPr>
@@ -68,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{7DD63EB1-A5C4-4504-91E7-16A6B6DB7D18}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{1E3537C5-B5CD-4A1E-853F-1D95D1F54CA4}">
       <text>
         <r>
           <rPr>
@@ -82,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{3384876E-CA5F-4C2C-821B-9110DF0F1381}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{5BD191EB-4549-4DD0-AA7D-AB704D108C1C}">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{C5305301-4922-46DD-BAD6-A5EE5AA03A46}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{4BCA141E-2121-47EC-B16F-EB950CC8F2FE}">
       <text>
         <r>
           <rPr>
@@ -110,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{DAF851A3-DCE5-4FE5-93AD-77EDC601DF51}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{95A0FAE8-2FB1-4E4D-A55A-954A43B61BDE}">
       <text>
         <r>
           <rPr>
@@ -134,7 +134,7 @@
     <author>Jorge Alejandro Falcon Alvarez</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{2A005B76-DA71-4550-87CB-33BD2F383206}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5AB12AC5-F074-4DA1-820F-FC306A57B6D2}">
       <text>
         <r>
           <rPr>
@@ -148,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{3C1BA7BC-BE40-4919-8866-914244E7777C}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{CE70417C-BE31-411E-81E7-99152221BED5}">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{B3ADD2FF-76EE-4BCD-84B7-19353002DA1E}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{C2B75E72-FD91-42ED-BDF2-9914041960C0}">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{151A7C4F-297D-4D4C-B0CA-616F2D52662C}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{42A23A84-4302-4876-AA5D-069707989ED0}">
       <text>
         <r>
           <rPr>
@@ -190,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{89976F48-A6D8-4E41-94DF-5F19A2824F62}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{ACAA097B-6B40-4DDD-ABB4-E0968CDF2EB0}">
       <text>
         <r>
           <rPr>
@@ -204,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{CEEBCCD0-3763-461B-8DAE-15FDB5125F19}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{8811A1CF-C0D5-4E4C-8012-DDD065D42B89}">
       <text>
         <r>
           <rPr>
@@ -218,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{F033482E-2640-439E-A30F-1C221C80C916}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{FC85BDEE-6452-4C85-AFB4-8F418B5AD0D5}">
       <text>
         <r>
           <rPr>
@@ -237,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="87">
   <si>
     <t>Nombre</t>
   </si>
@@ -269,37 +269,231 @@
     <t>Respuestas</t>
   </si>
   <si>
-    <t>Alvaro Fernández Ochoa</t>
-  </si>
-  <si>
-    <t>El error es que tiene el mismo nombre el archivo supongo.</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1409472/</t>
+    <t>Jorge Alejandro Falcon Alvarez</t>
+  </si>
+  <si>
+    <t>Posterior a la creación de la carpeta, debemos dar clic derecho sobre la carpeta, luego en Add y seleccionamos "Sequence" para crear el XAML. Otra forma de crear el XAML es dar clic derecho sobre la Sequence que tenemos en nuestro Main, luego elegimos "Extract as Workflow"</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408928/</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
     <t>Curso de Automatización de Procesos RPA con UiPath</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Jorge Alejandro Falcon Alvarez</t>
-  </si>
-  <si>
-    <t>Posterior a la creación de la carpeta, debemos dar clic derecho sobre la carpeta, luego en Add y seleccionamos "Sequence" para crear el XAML. Otra forma de crear el XAML es dar clic derecho sobre la Sequence que tenemos en nuestro Main, luego elegimos "Extract as Workflow"</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408928/</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Alvaro Fernández Ochoa</t>
+  </si>
+  <si>
+    <t>El error es que tiene el mismo nombre el archivo supongo.</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1409472/</t>
+  </si>
+  <si>
+    <t>eduardog89</t>
+  </si>
+  <si>
+    <t>espero mucho de este curso! me gustaria ser un especialisa en RPA</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408059/</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Contiene respuestas demasiado largas para ser soportadas en esta versión.</t>
+  </si>
+  <si>
+    <t>miniendo</t>
+  </si>
+  <si>
+    <t>Actualmente trabajo como Tester he tenido algo de contacto con procesos automatizados estoy anciancioso por aprender mas de procesos de automatizacio con esta herramienta y mejorar mi perfil profesional.</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406921/</t>
+  </si>
+  <si>
+    <t>Andres Felipe Bravo Piñeros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super!!! Trabajo con RPA a través de la herramienta Automation Anywhere pero estoy ansioso de aprender y empezar a trabajar con UiPath </t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406612/</t>
+  </si>
+  <si>
+    <t>jfespanolito : Welcome to the dark side.jpg</t>
+  </si>
+  <si>
+    <t>Lisa Daniela Villar Contreras</t>
+  </si>
+  <si>
+    <t>Esperaba mucho este curso ! Gracias</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406518/</t>
+  </si>
+  <si>
+    <t>Víctor León</t>
+  </si>
+  <si>
+    <t>Esperaba este curso</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406307/</t>
+  </si>
+  <si>
+    <t>Gonzalo Flores</t>
+  </si>
+  <si>
+    <t>Excelente, empezamos con toda la actitud</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406228/</t>
+  </si>
+  <si>
+    <t>German_Danilo_Forero</t>
+  </si>
+  <si>
+    <t>Explicación clara y prática, empezamos bien.</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406118/</t>
+  </si>
+  <si>
+    <t>Brayan Potosi Dominguez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que introducción tan innovadora </t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406091/</t>
+  </si>
+  <si>
+    <t>yeisonmmartinez</t>
+  </si>
+  <si>
+    <t>Sería bueno conocer cuáles artefactos genera cada rol para darle claridad a su aporte en el proceso</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1407719/</t>
+  </si>
+  <si>
+    <t>jfespanolito : Gracias por la recomendación, revisaré como integrarlo en esta clase.</t>
+  </si>
+  <si>
+    <t>Dario Perea</t>
+  </si>
+  <si>
+    <t>Como suele suceder en este hermoso ambiente. Tenemos la teoría, “lo ideal” y la práctica.
+Los roles están bien definidos y se debería respetar. Nada quita que el que releva el proceso, instale los programas, programe las tareas de ejecución y desarrolle, sea la misma persona. Es muy probable que una misma persona ocupe mas de un rol en el equipo. Al menos esa es la experiencia en nuestro equipo.</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1407232/</t>
+  </si>
+  <si>
+    <t>Alexander Silvera</t>
+  </si>
+  <si>
+    <t>Al parecer un desarrollador solo no podría crear por si solo este tipo de soluciones?? O es para procesos de automatización de alta escala donde participan todos estos actores???</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406337/</t>
+  </si>
+  <si>
+    <t>Muchos roles participantes en el proceso…</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406132/</t>
+  </si>
+  <si>
+    <t>me salen dos versiones… studio y studio X…una es la version de paga o algo asi?</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408105/</t>
+  </si>
+  <si>
+    <t>vamonos!</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408102/</t>
+  </si>
+  <si>
+    <t>En el siguiente enlace pueden verificar los requerimientos de Hardware y Software recomendados</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1407771/</t>
+  </si>
+  <si>
+    <t>No hay una guía de como descargar UiPathStudio para Ubuntu?? Porque no estoy pudiendo bajar el ejecutable.</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406657/</t>
+  </si>
+  <si>
+    <t>Perfecto, vamos a ello !</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406138/</t>
+  </si>
+  <si>
+    <t>Carlos Abel Dominguez Bautista</t>
+  </si>
+  <si>
+    <t>Brutal!</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408798/</t>
+  </si>
+  <si>
+    <t>todo listo hasta ahora…</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408159/</t>
+  </si>
+  <si>
+    <t>Con la versión community cómo se realiza el despliegue de un robot en producción?</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1407814/</t>
+  </si>
+  <si>
+    <t>Marcelo Ganin</t>
+  </si>
+  <si>
+    <t>Que diferencia hay entre la licencia de comunidad y una clave empresarial? funcionalidades? soporte?</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406205/</t>
+  </si>
+  <si>
+    <t>Así esta bien? me imagino que todavia no se sube todo el curso cierto? pero si este es el temario suena genial</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408207/</t>
+  </si>
+  <si>
+    <t>no se me creo automaticamente el archio EscribirHolaMundo.xaml … apesar que al ejecutar el robot si se ejecuto bien… tuve que realizarlo manualmente…porque a ti se te creo automaticamente el “XAML de Hola mundo” ?</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408315/</t>
+  </si>
+  <si>
     <t>victor rodriguez</t>
   </si>
   <si>
@@ -308,216 +502,6 @@
   </si>
   <si>
     <t>platzi.com/comentario/1409318/</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Contiene respuestas demasiado largas para ser soportadas en esta versión.</t>
-  </si>
-  <si>
-    <t>eduardog89</t>
-  </si>
-  <si>
-    <t>espero mucho de este curso! me gustaria ser un especialisa en RPA</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408059/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
-    <t>miniendo</t>
-  </si>
-  <si>
-    <t>Actualmente trabajo como Tester he tenido algo de contacto con procesos automatizados estoy anciancioso por aprender mas de procesos de automatizacio con esta herramienta y mejorar mi perfil profesional.</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406921/</t>
-  </si>
-  <si>
-    <t>Andres Felipe Bravo Piñeros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Super!!! Trabajo con RPA a través de la herramienta Automation Anywhere pero estoy ansioso de aprender y empezar a trabajar con UiPath </t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406612/</t>
-  </si>
-  <si>
-    <t>jfespanolito : Welcome to the dark side.jpg</t>
-  </si>
-  <si>
-    <t>Lisa Daniela Villar Contreras</t>
-  </si>
-  <si>
-    <t>Esperaba mucho este curso ! Gracias</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406518/</t>
-  </si>
-  <si>
-    <t>Víctor León</t>
-  </si>
-  <si>
-    <t>Esperaba este curso</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406307/</t>
-  </si>
-  <si>
-    <t>Gonzalo Flores</t>
-  </si>
-  <si>
-    <t>Excelente, empezamos con toda la actitud</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406228/</t>
-  </si>
-  <si>
-    <t>German_Danilo_Forero</t>
-  </si>
-  <si>
-    <t>Explicación clara y prática, empezamos bien.</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406118/</t>
-  </si>
-  <si>
-    <t>Brayan Potosi Dominguez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Que introducción tan innovadora </t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406091/</t>
-  </si>
-  <si>
-    <t>yeisonmmartinez</t>
-  </si>
-  <si>
-    <t>Sería bueno conocer cuáles artefactos genera cada rol para darle claridad a su aporte en el proceso</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1407719/</t>
-  </si>
-  <si>
-    <t>jfespanolito : Gracias por la recomendación, revisaré como integrarlo en esta clase.</t>
-  </si>
-  <si>
-    <t>Dario Perea</t>
-  </si>
-  <si>
-    <t>Como suele suceder en este hermoso ambiente. Tenemos la teoría, “lo ideal” y la práctica.
-Los roles están bien definidos y se debería respetar. Nada quita que el que releva el proceso, instale los programas, programe las tareas de ejecución y desarrolle, sea la misma persona. Es muy probable que una misma persona ocupe mas de un rol en el equipo. Al menos esa es la experiencia en nuestro equipo.</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1407232/</t>
-  </si>
-  <si>
-    <t>Alexander Silvera</t>
-  </si>
-  <si>
-    <t>Al parecer un desarrollador solo no podría crear por si solo este tipo de soluciones?? O es para procesos de automatización de alta escala donde participan todos estos actores???</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406337/</t>
-  </si>
-  <si>
-    <t>Muchos roles participantes en el proceso…</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406132/</t>
-  </si>
-  <si>
-    <t>me salen dos versiones… studio y studio X…una es la version de paga o algo asi?</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408105/</t>
-  </si>
-  <si>
-    <t>vamonos!</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408102/</t>
-  </si>
-  <si>
-    <t>En el siguiente enlace pueden verificar los requerimientos de Hardware y Software recomendados</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1407771/</t>
-  </si>
-  <si>
-    <t>No hay una guía de como descargar UiPathStudio para Ubuntu?? Porque no estoy pudiendo bajar el ejecutable.</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406657/</t>
-  </si>
-  <si>
-    <t>Perfecto, vamos a ello !</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406138/</t>
-  </si>
-  <si>
-    <t>Carlos Abel Dominguez Bautista</t>
-  </si>
-  <si>
-    <t>Brutal!</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408798/</t>
-  </si>
-  <si>
-    <t>todo listo hasta ahora…</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408159/</t>
-  </si>
-  <si>
-    <t>Con la versión community cómo se realiza el despliegue de un robot en producción?</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1407814/</t>
-  </si>
-  <si>
-    <t>Marcelo Ganin</t>
-  </si>
-  <si>
-    <t>Que diferencia hay entre la licencia de comunidad y una clave empresarial? funcionalidades? soporte?</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406205/</t>
-  </si>
-  <si>
-    <t>Así esta bien? me imagino que todavia no se sube todo el curso cierto? pero si este es el temario suena genial</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408207/</t>
-  </si>
-  <si>
-    <t>no se me creo automaticamente el archio EscribirHolaMundo.xaml … apesar que al ejecutar el robot si se ejecuto bien… tuve que realizarlo manualmente…porque a ti se te creo automaticamente el “XAML de Hola mundo” ?</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408315/</t>
-  </si>
-  <si>
-    <t>Nicolas Antognoli</t>
-  </si>
-  <si>
-    <t>Actualmente donde trabajo usamos UIPath para la carga de facturas de proveedores y funciona perfecto el OCR leyendo las mismas. Y cuando algún dato no encuentra pregunta por mail para continuar con la carga. Tambien para cargar datos de tipo de cambio a los sistemas, conciliaciones bancarias, etc.etc… Yo creo que lo mejor es comenzar con procesos chicos, y luego ir agarrando impulso con proyectos mas grandes, para que entiendan el potencial de la herramienta. El miedo al reemplazo a veces genera que no se abran para estas tecnologías, pero en realidad tienen que convivir ambas, y donde se generan procesos repetitivos dar lugar al RPA para que las personas se enfoquen mas en temas de análisis.</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406404/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
-  </si>
-  <si>
-    <t>jfespanolito : Así es, hay que convivir y crecer poco a poco… Gran recomendación, gracias por ella.</t>
   </si>
 </sst>
 </file>
@@ -919,7 +903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -935,11 +919,14 @@
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -955,19 +942,22 @@
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -976,21 +966,21 @@
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -999,10 +989,10 @@
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1013,7 +1003,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1063,7 +1053,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1079,22 +1069,25 @@
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>23</v>
@@ -1102,22 +1095,22 @@
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>23</v>
@@ -1126,24 +1119,24 @@
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>23</v>
@@ -1152,21 +1145,21 @@
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>23</v>
@@ -1175,24 +1168,21 @@
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>23</v>
@@ -1201,21 +1191,21 @@
         <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
@@ -1224,21 +1214,21 @@
         <v>14</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>23</v>
@@ -1247,21 +1237,21 @@
         <v>14</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>23</v>
@@ -1270,22 +1260,25 @@
         <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1293,21 +1286,21 @@
         <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>23</v>
@@ -1316,24 +1309,24 @@
         <v>14</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>23</v>
@@ -1342,21 +1335,21 @@
         <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>23</v>
@@ -1365,24 +1358,21 @@
         <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>23</v>
@@ -1391,21 +1381,21 @@
         <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>23</v>
@@ -1414,21 +1404,21 @@
         <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>23</v>
@@ -1437,21 +1427,21 @@
         <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>23</v>
@@ -1460,21 +1450,24 @@
         <v>14</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>23</v>
@@ -1483,21 +1476,21 @@
         <v>14</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>23</v>
@@ -1506,24 +1499,24 @@
         <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>23</v>
@@ -1532,21 +1525,21 @@
         <v>14</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>23</v>
@@ -1555,24 +1548,24 @@
         <v>14</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>23</v>
@@ -1581,70 +1574,73 @@
         <v>14</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>23</v>
@@ -1653,24 +1649,21 @@
         <v>14</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>23</v>
@@ -1679,24 +1672,21 @@
         <v>14</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>23</v>
@@ -1705,21 +1695,21 @@
         <v>14</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>23</v>
@@ -1728,21 +1718,21 @@
         <v>14</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>23</v>
@@ -1751,21 +1741,21 @@
         <v>14</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>23</v>
@@ -1774,44 +1764,50 @@
         <v>14</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>23</v>
@@ -1820,70 +1816,70 @@
         <v>14</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="1" t="s">
+    </row>
+    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>85</v>
@@ -1898,18 +1894,18 @@
         <v>14</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>85</v>
@@ -1924,39 +1920,13 @@
         <v>14</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se corrige sistema de eliminación de duplicados.
</commit_message>
<xml_diff>
--- a/Archivos/Comentarios.xlsx
+++ b/Archivos/Comentarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_3073F1A66CECAA25EA8A224031E1565DDEC81B98" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{24576135-35A4-442F-A378-720D5F1D161B}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="11_A08F948C58EDAA75EA164C92AAC48A17F3D0AC1C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2C957209-0087-4A8A-BCC3-475DCD9AD64A}"/>
   <bookViews>
-    <workbookView xWindow="30975" yWindow="1380" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30825" yWindow="1710" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nuevos" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <author>Jorge Alejandro Falcon Alvarez</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{4658A65F-C538-4F06-813B-F4B39DF2C7A3}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{1371EE71-2DE5-4005-87A0-65C5F6FDF720}">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{3253681F-4806-4A72-982F-3B8E314D87A8}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{81F2AE60-D525-466C-B076-4DD949AB6DD1}">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{814A1CC0-BEC1-4CA0-8E33-452FB41321C3}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{4E414DBB-C140-4E44-808C-327671B5951C}">
       <text>
         <r>
           <rPr>
@@ -68,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{1E3537C5-B5CD-4A1E-853F-1D95D1F54CA4}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{47A9ED7C-79EE-459B-9951-C3EBD3A9BE12}">
       <text>
         <r>
           <rPr>
@@ -82,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{5BD191EB-4549-4DD0-AA7D-AB704D108C1C}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{9F6AC247-385C-4AA8-BB08-3D24D58D35DA}">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{4BCA141E-2121-47EC-B16F-EB950CC8F2FE}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{5BC8DBE8-76C0-4B3D-9E27-0608AD491174}">
       <text>
         <r>
           <rPr>
@@ -110,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{95A0FAE8-2FB1-4E4D-A55A-954A43B61BDE}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{AF72F395-8D53-4692-A1F5-FBB38FAEF64F}">
       <text>
         <r>
           <rPr>
@@ -134,7 +134,7 @@
     <author>Jorge Alejandro Falcon Alvarez</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5AB12AC5-F074-4DA1-820F-FC306A57B6D2}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{98EF5229-973F-42FD-99E4-320641C30DF6}">
       <text>
         <r>
           <rPr>
@@ -148,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{CE70417C-BE31-411E-81E7-99152221BED5}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6CB562D5-2484-444D-A232-388958DA2738}">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{C2B75E72-FD91-42ED-BDF2-9914041960C0}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{39EF70E1-8970-4386-8FDD-F5DC2D4EEEBF}">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{42A23A84-4302-4876-AA5D-069707989ED0}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D821D7CA-4FC1-42A1-AF62-9B8010568551}">
       <text>
         <r>
           <rPr>
@@ -190,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{ACAA097B-6B40-4DDD-ABB4-E0968CDF2EB0}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{552BB6FB-3075-4633-AB2B-4CB4B160814E}">
       <text>
         <r>
           <rPr>
@@ -204,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{8811A1CF-C0D5-4E4C-8012-DDD065D42B89}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{6EBA2DFB-AE2A-41DB-91E3-5EF3853E9E83}">
       <text>
         <r>
           <rPr>
@@ -218,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{FC85BDEE-6452-4C85-AFB4-8F418B5AD0D5}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{9D5CF698-E6F9-4CEF-84C9-4B9F97C1EAA8}">
       <text>
         <r>
           <rPr>
@@ -237,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="89">
   <si>
     <t>Nombre</t>
   </si>
@@ -300,13 +300,13 @@
     <t>platzi.com/comentario/1409472/</t>
   </si>
   <si>
-    <t>eduardog89</t>
-  </si>
-  <si>
-    <t>espero mucho de este curso! me gustaria ser un especialisa en RPA</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1408059/</t>
+    <t>miniendo</t>
+  </si>
+  <si>
+    <t>Actualmente trabajo como Tester he tenido algo de contacto con procesos automatizados estoy anciancioso por aprender mas de procesos de automatizacio con esta herramienta y mejorar mi perfil profesional.</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1406921/</t>
   </si>
   <si>
     <t>2</t>
@@ -316,18 +316,6 @@
 </t>
   </si>
   <si>
-    <t>Contiene respuestas demasiado largas para ser soportadas en esta versión.</t>
-  </si>
-  <si>
-    <t>miniendo</t>
-  </si>
-  <si>
-    <t>Actualmente trabajo como Tester he tenido algo de contacto con procesos automatizados estoy anciancioso por aprender mas de procesos de automatizacio con esta herramienta y mejorar mi perfil profesional.</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1406921/</t>
-  </si>
-  <si>
     <t>Andres Felipe Bravo Piñeros</t>
   </si>
   <si>
@@ -383,18 +371,6 @@
   </si>
   <si>
     <t>platzi.com/comentario/1406091/</t>
-  </si>
-  <si>
-    <t>yeisonmmartinez</t>
-  </si>
-  <si>
-    <t>Sería bueno conocer cuáles artefactos genera cada rol para darle claridad a su aporte en el proceso</t>
-  </si>
-  <si>
-    <t>platzi.com/comentario/1407719/</t>
-  </si>
-  <si>
-    <t>jfespanolito : Gracias por la recomendación, revisaré como integrarlo en esta clase.</t>
   </si>
   <si>
     <t>Dario Perea</t>
@@ -407,6 +383,10 @@
     <t>platzi.com/comentario/1407232/</t>
   </si>
   <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
     <t>Alexander Silvera</t>
   </si>
   <si>
@@ -416,12 +396,18 @@
     <t>platzi.com/comentario/1406337/</t>
   </si>
   <si>
+    <t>Contiene respuestas demasiado largas para ser soportadas en esta versión.</t>
+  </si>
+  <si>
     <t>Muchos roles participantes en el proceso…</t>
   </si>
   <si>
     <t>platzi.com/comentario/1406132/</t>
   </si>
   <si>
+    <t>eduardog89</t>
+  </si>
+  <si>
     <t>me salen dos versiones… studio y studio X…una es la version de paga o algo asi?</t>
   </si>
   <si>
@@ -432,6 +418,9 @@
   </si>
   <si>
     <t>platzi.com/comentario/1408102/</t>
+  </si>
+  <si>
+    <t>yeisonmmartinez</t>
   </si>
   <si>
     <t>En el siguiente enlace pueden verificar los requerimientos de Hardware y Software recomendados</t>
@@ -502,6 +491,24 @@
   </si>
   <si>
     <t>platzi.com/comentario/1409318/</t>
+  </si>
+  <si>
+    <t>espero mucho de este curso! me gustaria ser un especialisa en RPA</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1408059/</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Sería bueno conocer cuáles artefactos genera cada rol para darle claridad a su aporte en el proceso</t>
+  </si>
+  <si>
+    <t>platzi.com/comentario/1407719/</t>
+  </si>
+  <si>
+    <t>jfespanolito : Gracias por la recomendación, revisaré como integrarlo en esta clase.</t>
   </si>
 </sst>
 </file>
@@ -853,7 +860,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -903,7 +910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -926,15 +933,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -946,52 +953,6 @@
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1003,7 +964,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1053,7 +1014,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1075,19 +1036,16 @@
       <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>23</v>
@@ -1101,8 +1059,11 @@
       <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1124,19 +1085,16 @@
       <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>23</v>
@@ -1151,15 +1109,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>23</v>
@@ -1174,15 +1132,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>23</v>
@@ -1197,15 +1155,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
@@ -1220,38 +1178,38 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>23</v>
@@ -1260,24 +1218,24 @@
         <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>23</v>
@@ -1286,21 +1244,21 @@
         <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>23</v>
@@ -1309,24 +1267,24 @@
         <v>14</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>23</v>
@@ -1335,67 +1293,73 @@
         <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>23</v>
@@ -1404,21 +1368,21 @@
         <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>23</v>
@@ -1433,15 +1397,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>23</v>
@@ -1455,42 +1419,42 @@
       <c r="G18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="1" t="s">
+    </row>
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>23</v>
@@ -1499,24 +1463,24 @@
         <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>23</v>
@@ -1525,21 +1489,24 @@
         <v>14</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="J21" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>23</v>
@@ -1554,18 +1521,18 @@
         <v>16</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>23</v>
@@ -1579,19 +1546,22 @@
       <c r="G23" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="J23" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
@@ -1603,330 +1573,33 @@
         <v>16</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>